<commit_message>
added lecture 4 of LOT course
</commit_message>
<xml_diff>
--- a/content/resources/corpora/minimal-stress-pairs.xlsx
+++ b/content/resources/corpora/minimal-stress-pairs.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20410"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20411"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\CYOD-ADMIN\Documents\git\hrbosker.github.io\content\resources\corpora\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{31981EAA-81A9-4AEC-986D-708417DD53A4}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AB742F31-B917-402D-BC7D-198153F706DB}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="8010" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2699" uniqueCount="1804">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2704" uniqueCount="1808">
   <si>
     <t>Word 1</t>
   </si>
@@ -5989,6 +5989,18 @@
   </si>
   <si>
     <t>Comments</t>
+  </si>
+  <si>
+    <t>achterwegen</t>
+  </si>
+  <si>
+    <t>back roads</t>
+  </si>
+  <si>
+    <t>achterwege</t>
+  </si>
+  <si>
+    <t>omitted/left out (adv.)</t>
   </si>
 </sst>
 </file>
@@ -6803,9 +6815,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{09BD612E-4F01-4431-B7ED-538D524FB554}">
-  <dimension ref="A1:I101"/>
+  <dimension ref="A1:I102"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="A78" workbookViewId="0">
+      <selection activeCell="H87" sqref="H87"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
@@ -9004,25 +9018,25 @@
         <v>4</v>
       </c>
       <c r="B87" s="43" t="s">
-        <v>1548</v>
+        <v>1804</v>
       </c>
       <c r="C87" s="44">
         <v>1</v>
       </c>
       <c r="D87" s="44" t="s">
-        <v>1560</v>
+        <v>1805</v>
       </c>
       <c r="E87" s="45" t="s">
         <v>1211</v>
       </c>
       <c r="F87" s="43" t="s">
-        <v>1548</v>
+        <v>1806</v>
       </c>
       <c r="G87" s="44">
         <v>3</v>
       </c>
       <c r="H87" s="44" t="s">
-        <v>1561</v>
+        <v>1807</v>
       </c>
       <c r="I87" s="91"/>
     </row>
@@ -9031,25 +9045,25 @@
         <v>4</v>
       </c>
       <c r="B88" s="43" t="s">
-        <v>1769</v>
+        <v>1548</v>
       </c>
       <c r="C88" s="44">
         <v>1</v>
       </c>
       <c r="D88" s="44" t="s">
-        <v>1776</v>
+        <v>1560</v>
       </c>
       <c r="E88" s="45" t="s">
         <v>1211</v>
       </c>
       <c r="F88" s="43" t="s">
-        <v>1769</v>
+        <v>1548</v>
       </c>
       <c r="G88" s="44">
         <v>3</v>
       </c>
       <c r="H88" s="44" t="s">
-        <v>1775</v>
+        <v>1561</v>
       </c>
       <c r="I88" s="91"/>
     </row>
@@ -9058,57 +9072,55 @@
         <v>4</v>
       </c>
       <c r="B89" s="43" t="s">
-        <v>1616</v>
+        <v>1769</v>
       </c>
       <c r="C89" s="44">
         <v>1</v>
       </c>
       <c r="D89" s="44" t="s">
-        <v>1687</v>
+        <v>1776</v>
       </c>
       <c r="E89" s="45" t="s">
         <v>1211</v>
       </c>
       <c r="F89" s="43" t="s">
-        <v>1616</v>
+        <v>1769</v>
       </c>
       <c r="G89" s="44">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="H89" s="44" t="s">
-        <v>1689</v>
-      </c>
-      <c r="I89" s="91" t="s">
-        <v>1700</v>
-      </c>
+        <v>1775</v>
+      </c>
+      <c r="I89" s="91"/>
     </row>
     <row r="90" spans="1:9" s="44" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A90" s="42">
         <v>4</v>
       </c>
       <c r="B90" s="43" t="s">
-        <v>582</v>
+        <v>1616</v>
       </c>
       <c r="C90" s="44">
         <v>1</v>
       </c>
       <c r="D90" s="44" t="s">
-        <v>616</v>
+        <v>1687</v>
       </c>
       <c r="E90" s="45" t="s">
         <v>1211</v>
       </c>
       <c r="F90" s="43" t="s">
-        <v>582</v>
+        <v>1616</v>
       </c>
       <c r="G90" s="44">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="H90" s="44" t="s">
-        <v>635</v>
+        <v>1689</v>
       </c>
       <c r="I90" s="91" t="s">
-        <v>1701</v>
+        <v>1700</v>
       </c>
     </row>
     <row r="91" spans="1:9" s="44" customFormat="1" x14ac:dyDescent="0.35">
@@ -9116,25 +9128,25 @@
         <v>4</v>
       </c>
       <c r="B91" s="43" t="s">
-        <v>1634</v>
+        <v>582</v>
       </c>
       <c r="C91" s="44">
         <v>1</v>
       </c>
       <c r="D91" s="44" t="s">
-        <v>1697</v>
+        <v>616</v>
       </c>
       <c r="E91" s="45" t="s">
         <v>1211</v>
       </c>
       <c r="F91" s="43" t="s">
-        <v>1634</v>
+        <v>582</v>
       </c>
       <c r="G91" s="44">
         <v>3</v>
       </c>
       <c r="H91" s="44" t="s">
-        <v>1698</v>
+        <v>635</v>
       </c>
       <c r="I91" s="91" t="s">
         <v>1701</v>
@@ -9145,28 +9157,28 @@
         <v>4</v>
       </c>
       <c r="B92" s="43" t="s">
-        <v>1615</v>
+        <v>1634</v>
       </c>
       <c r="C92" s="44">
         <v>1</v>
       </c>
       <c r="D92" s="44" t="s">
-        <v>1690</v>
+        <v>1697</v>
       </c>
       <c r="E92" s="45" t="s">
         <v>1211</v>
       </c>
       <c r="F92" s="43" t="s">
-        <v>1615</v>
+        <v>1634</v>
       </c>
       <c r="G92" s="44">
         <v>3</v>
       </c>
       <c r="H92" s="44" t="s">
-        <v>1699</v>
+        <v>1698</v>
       </c>
       <c r="I92" s="91" t="s">
-        <v>1628</v>
+        <v>1701</v>
       </c>
     </row>
     <row r="93" spans="1:9" s="44" customFormat="1" x14ac:dyDescent="0.35">
@@ -9174,28 +9186,28 @@
         <v>4</v>
       </c>
       <c r="B93" s="43" t="s">
-        <v>1620</v>
+        <v>1615</v>
       </c>
       <c r="C93" s="44">
         <v>1</v>
       </c>
       <c r="D93" s="44" t="s">
-        <v>1682</v>
+        <v>1690</v>
       </c>
       <c r="E93" s="45" t="s">
         <v>1211</v>
       </c>
       <c r="F93" s="43" t="s">
-        <v>1683</v>
+        <v>1615</v>
       </c>
       <c r="G93" s="44">
         <v>3</v>
       </c>
       <c r="H93" s="44" t="s">
-        <v>1685</v>
+        <v>1699</v>
       </c>
       <c r="I93" s="91" t="s">
-        <v>1702</v>
+        <v>1628</v>
       </c>
     </row>
     <row r="94" spans="1:9" s="44" customFormat="1" x14ac:dyDescent="0.35">
@@ -9203,28 +9215,28 @@
         <v>4</v>
       </c>
       <c r="B94" s="43" t="s">
-        <v>1545</v>
+        <v>1620</v>
       </c>
       <c r="C94" s="44">
         <v>1</v>
       </c>
       <c r="D94" s="44" t="s">
-        <v>1567</v>
+        <v>1682</v>
       </c>
       <c r="E94" s="45" t="s">
         <v>1211</v>
       </c>
       <c r="F94" s="43" t="s">
-        <v>1545</v>
+        <v>1683</v>
       </c>
       <c r="G94" s="44">
         <v>3</v>
       </c>
       <c r="H94" s="44" t="s">
-        <v>1568</v>
+        <v>1685</v>
       </c>
       <c r="I94" s="91" t="s">
-        <v>1672</v>
+        <v>1702</v>
       </c>
     </row>
     <row r="95" spans="1:9" s="44" customFormat="1" x14ac:dyDescent="0.35">
@@ -9232,25 +9244,25 @@
         <v>4</v>
       </c>
       <c r="B95" s="43" t="s">
-        <v>1640</v>
+        <v>1545</v>
       </c>
       <c r="C95" s="44">
         <v>1</v>
       </c>
       <c r="D95" s="44" t="s">
-        <v>1691</v>
+        <v>1567</v>
       </c>
       <c r="E95" s="45" t="s">
         <v>1211</v>
       </c>
       <c r="F95" s="43" t="s">
-        <v>1640</v>
+        <v>1545</v>
       </c>
       <c r="G95" s="44">
         <v>3</v>
       </c>
       <c r="H95" s="44" t="s">
-        <v>1692</v>
+        <v>1568</v>
       </c>
       <c r="I95" s="91" t="s">
         <v>1672</v>
@@ -9261,28 +9273,28 @@
         <v>4</v>
       </c>
       <c r="B96" s="43" t="s">
-        <v>1547</v>
+        <v>1640</v>
       </c>
       <c r="C96" s="44">
         <v>1</v>
       </c>
       <c r="D96" s="44" t="s">
-        <v>1562</v>
+        <v>1691</v>
       </c>
       <c r="E96" s="45" t="s">
         <v>1211</v>
       </c>
       <c r="F96" s="43" t="s">
-        <v>1547</v>
+        <v>1640</v>
       </c>
       <c r="G96" s="44">
         <v>3</v>
       </c>
       <c r="H96" s="44" t="s">
-        <v>1563</v>
+        <v>1692</v>
       </c>
       <c r="I96" s="91" t="s">
-        <v>1673</v>
+        <v>1672</v>
       </c>
     </row>
     <row r="97" spans="1:9" s="44" customFormat="1" x14ac:dyDescent="0.35">
@@ -9290,25 +9302,25 @@
         <v>4</v>
       </c>
       <c r="B97" s="43" t="s">
-        <v>1637</v>
+        <v>1547</v>
       </c>
       <c r="C97" s="44">
         <v>1</v>
       </c>
       <c r="D97" s="44" t="s">
-        <v>1695</v>
+        <v>1562</v>
       </c>
       <c r="E97" s="45" t="s">
         <v>1211</v>
       </c>
       <c r="F97" s="43" t="s">
-        <v>1637</v>
+        <v>1547</v>
       </c>
       <c r="G97" s="44">
         <v>3</v>
       </c>
       <c r="H97" s="44" t="s">
-        <v>1696</v>
+        <v>1563</v>
       </c>
       <c r="I97" s="91" t="s">
         <v>1673</v>
@@ -9319,28 +9331,28 @@
         <v>4</v>
       </c>
       <c r="B98" s="43" t="s">
-        <v>1621</v>
+        <v>1637</v>
       </c>
       <c r="C98" s="44">
         <v>1</v>
       </c>
       <c r="D98" s="44" t="s">
-        <v>1693</v>
+        <v>1695</v>
       </c>
       <c r="E98" s="45" t="s">
         <v>1211</v>
       </c>
       <c r="F98" s="43" t="s">
-        <v>1621</v>
+        <v>1637</v>
       </c>
       <c r="G98" s="44">
         <v>3</v>
       </c>
       <c r="H98" s="44" t="s">
-        <v>1694</v>
+        <v>1696</v>
       </c>
       <c r="I98" s="91" t="s">
-        <v>1703</v>
+        <v>1673</v>
       </c>
     </row>
     <row r="99" spans="1:9" s="44" customFormat="1" x14ac:dyDescent="0.35">
@@ -9348,28 +9360,28 @@
         <v>4</v>
       </c>
       <c r="B99" s="43" t="s">
-        <v>1595</v>
+        <v>1621</v>
       </c>
       <c r="C99" s="44">
         <v>1</v>
       </c>
       <c r="D99" s="44" t="s">
-        <v>1596</v>
+        <v>1693</v>
       </c>
       <c r="E99" s="45" t="s">
         <v>1211</v>
       </c>
       <c r="F99" s="43" t="s">
-        <v>1598</v>
+        <v>1621</v>
       </c>
       <c r="G99" s="44">
         <v>3</v>
       </c>
       <c r="H99" s="44" t="s">
-        <v>1599</v>
+        <v>1694</v>
       </c>
       <c r="I99" s="91" t="s">
-        <v>1704</v>
+        <v>1703</v>
       </c>
     </row>
     <row r="100" spans="1:9" s="44" customFormat="1" x14ac:dyDescent="0.35">
@@ -9377,32 +9389,61 @@
         <v>4</v>
       </c>
       <c r="B100" s="43" t="s">
-        <v>604</v>
+        <v>1595</v>
       </c>
       <c r="C100" s="44">
         <v>1</v>
       </c>
       <c r="D100" s="44" t="s">
-        <v>639</v>
+        <v>1596</v>
       </c>
       <c r="E100" s="45" t="s">
         <v>1211</v>
       </c>
       <c r="F100" s="43" t="s">
+        <v>1598</v>
+      </c>
+      <c r="G100" s="44">
+        <v>3</v>
+      </c>
+      <c r="H100" s="44" t="s">
+        <v>1599</v>
+      </c>
+      <c r="I100" s="91" t="s">
+        <v>1704</v>
+      </c>
+    </row>
+    <row r="101" spans="1:9" s="44" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A101" s="42">
+        <v>4</v>
+      </c>
+      <c r="B101" s="43" t="s">
         <v>604</v>
       </c>
-      <c r="G100" s="44">
-        <v>3</v>
-      </c>
-      <c r="H100" s="44" t="s">
+      <c r="C101" s="44">
+        <v>1</v>
+      </c>
+      <c r="D101" s="44" t="s">
+        <v>639</v>
+      </c>
+      <c r="E101" s="45" t="s">
+        <v>1211</v>
+      </c>
+      <c r="F101" s="43" t="s">
+        <v>604</v>
+      </c>
+      <c r="G101" s="44">
+        <v>3</v>
+      </c>
+      <c r="H101" s="44" t="s">
         <v>644</v>
       </c>
-      <c r="I100" s="91" t="s">
+      <c r="I101" s="91" t="s">
         <v>1614</v>
       </c>
     </row>
-    <row r="101" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="B101" s="33"/>
+    <row r="102" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="B102" s="33"/>
     </row>
   </sheetData>
   <hyperlinks>

</xml_diff>

<commit_message>
created alumni category and added podcast newsitem
</commit_message>
<xml_diff>
--- a/content/resources/corpora/minimal-stress-pairs.xlsx
+++ b/content/resources/corpora/minimal-stress-pairs.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\CYOD-ADMIN\Documents\git\hrbosker.github.io\content\resources\corpora\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AB742F31-B917-402D-BC7D-198153F706DB}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D6788C12-C553-4347-BB76-D7D03EBE01F6}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="8010" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2704" uniqueCount="1808">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2709" uniqueCount="1811">
   <si>
     <t>Word 1</t>
   </si>
@@ -6001,6 +6001,15 @@
   </si>
   <si>
     <t>omitted/left out (adv.)</t>
+  </si>
+  <si>
+    <t>misdadiger</t>
+  </si>
+  <si>
+    <t>criminal (noun)</t>
+  </si>
+  <si>
+    <t>more felonious</t>
   </si>
 </sst>
 </file>
@@ -6815,11 +6824,9 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{09BD612E-4F01-4431-B7ED-538D524FB554}">
-  <dimension ref="A1:I102"/>
+  <dimension ref="A1:I103"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A78" workbookViewId="0">
-      <selection activeCell="H87" sqref="H87"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
@@ -9018,25 +9025,25 @@
         <v>4</v>
       </c>
       <c r="B87" s="43" t="s">
-        <v>1804</v>
+        <v>1808</v>
       </c>
       <c r="C87" s="44">
         <v>1</v>
       </c>
       <c r="D87" s="44" t="s">
-        <v>1805</v>
+        <v>1809</v>
       </c>
       <c r="E87" s="45" t="s">
         <v>1211</v>
       </c>
       <c r="F87" s="43" t="s">
-        <v>1806</v>
+        <v>1808</v>
       </c>
       <c r="G87" s="44">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="H87" s="44" t="s">
-        <v>1807</v>
+        <v>1810</v>
       </c>
       <c r="I87" s="91"/>
     </row>
@@ -9045,25 +9052,25 @@
         <v>4</v>
       </c>
       <c r="B88" s="43" t="s">
-        <v>1548</v>
+        <v>1804</v>
       </c>
       <c r="C88" s="44">
         <v>1</v>
       </c>
       <c r="D88" s="44" t="s">
-        <v>1560</v>
+        <v>1805</v>
       </c>
       <c r="E88" s="45" t="s">
         <v>1211</v>
       </c>
       <c r="F88" s="43" t="s">
-        <v>1548</v>
+        <v>1806</v>
       </c>
       <c r="G88" s="44">
         <v>3</v>
       </c>
       <c r="H88" s="44" t="s">
-        <v>1561</v>
+        <v>1807</v>
       </c>
       <c r="I88" s="91"/>
     </row>
@@ -9072,25 +9079,25 @@
         <v>4</v>
       </c>
       <c r="B89" s="43" t="s">
-        <v>1769</v>
+        <v>1548</v>
       </c>
       <c r="C89" s="44">
         <v>1</v>
       </c>
       <c r="D89" s="44" t="s">
-        <v>1776</v>
+        <v>1560</v>
       </c>
       <c r="E89" s="45" t="s">
         <v>1211</v>
       </c>
       <c r="F89" s="43" t="s">
-        <v>1769</v>
+        <v>1548</v>
       </c>
       <c r="G89" s="44">
         <v>3</v>
       </c>
       <c r="H89" s="44" t="s">
-        <v>1775</v>
+        <v>1561</v>
       </c>
       <c r="I89" s="91"/>
     </row>
@@ -9099,57 +9106,55 @@
         <v>4</v>
       </c>
       <c r="B90" s="43" t="s">
-        <v>1616</v>
+        <v>1769</v>
       </c>
       <c r="C90" s="44">
         <v>1</v>
       </c>
       <c r="D90" s="44" t="s">
-        <v>1687</v>
+        <v>1776</v>
       </c>
       <c r="E90" s="45" t="s">
         <v>1211</v>
       </c>
       <c r="F90" s="43" t="s">
-        <v>1616</v>
+        <v>1769</v>
       </c>
       <c r="G90" s="44">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="H90" s="44" t="s">
-        <v>1689</v>
-      </c>
-      <c r="I90" s="91" t="s">
-        <v>1700</v>
-      </c>
+        <v>1775</v>
+      </c>
+      <c r="I90" s="91"/>
     </row>
     <row r="91" spans="1:9" s="44" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A91" s="42">
         <v>4</v>
       </c>
       <c r="B91" s="43" t="s">
-        <v>582</v>
+        <v>1616</v>
       </c>
       <c r="C91" s="44">
         <v>1</v>
       </c>
       <c r="D91" s="44" t="s">
-        <v>616</v>
+        <v>1687</v>
       </c>
       <c r="E91" s="45" t="s">
         <v>1211</v>
       </c>
       <c r="F91" s="43" t="s">
-        <v>582</v>
+        <v>1616</v>
       </c>
       <c r="G91" s="44">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="H91" s="44" t="s">
-        <v>635</v>
+        <v>1689</v>
       </c>
       <c r="I91" s="91" t="s">
-        <v>1701</v>
+        <v>1700</v>
       </c>
     </row>
     <row r="92" spans="1:9" s="44" customFormat="1" x14ac:dyDescent="0.35">
@@ -9157,25 +9162,25 @@
         <v>4</v>
       </c>
       <c r="B92" s="43" t="s">
-        <v>1634</v>
+        <v>582</v>
       </c>
       <c r="C92" s="44">
         <v>1</v>
       </c>
       <c r="D92" s="44" t="s">
-        <v>1697</v>
+        <v>616</v>
       </c>
       <c r="E92" s="45" t="s">
         <v>1211</v>
       </c>
       <c r="F92" s="43" t="s">
-        <v>1634</v>
+        <v>582</v>
       </c>
       <c r="G92" s="44">
         <v>3</v>
       </c>
       <c r="H92" s="44" t="s">
-        <v>1698</v>
+        <v>635</v>
       </c>
       <c r="I92" s="91" t="s">
         <v>1701</v>
@@ -9186,28 +9191,28 @@
         <v>4</v>
       </c>
       <c r="B93" s="43" t="s">
-        <v>1615</v>
+        <v>1634</v>
       </c>
       <c r="C93" s="44">
         <v>1</v>
       </c>
       <c r="D93" s="44" t="s">
-        <v>1690</v>
+        <v>1697</v>
       </c>
       <c r="E93" s="45" t="s">
         <v>1211</v>
       </c>
       <c r="F93" s="43" t="s">
-        <v>1615</v>
+        <v>1634</v>
       </c>
       <c r="G93" s="44">
         <v>3</v>
       </c>
       <c r="H93" s="44" t="s">
-        <v>1699</v>
+        <v>1698</v>
       </c>
       <c r="I93" s="91" t="s">
-        <v>1628</v>
+        <v>1701</v>
       </c>
     </row>
     <row r="94" spans="1:9" s="44" customFormat="1" x14ac:dyDescent="0.35">
@@ -9215,28 +9220,28 @@
         <v>4</v>
       </c>
       <c r="B94" s="43" t="s">
-        <v>1620</v>
+        <v>1615</v>
       </c>
       <c r="C94" s="44">
         <v>1</v>
       </c>
       <c r="D94" s="44" t="s">
-        <v>1682</v>
+        <v>1690</v>
       </c>
       <c r="E94" s="45" t="s">
         <v>1211</v>
       </c>
       <c r="F94" s="43" t="s">
-        <v>1683</v>
+        <v>1615</v>
       </c>
       <c r="G94" s="44">
         <v>3</v>
       </c>
       <c r="H94" s="44" t="s">
-        <v>1685</v>
+        <v>1699</v>
       </c>
       <c r="I94" s="91" t="s">
-        <v>1702</v>
+        <v>1628</v>
       </c>
     </row>
     <row r="95" spans="1:9" s="44" customFormat="1" x14ac:dyDescent="0.35">
@@ -9244,28 +9249,28 @@
         <v>4</v>
       </c>
       <c r="B95" s="43" t="s">
-        <v>1545</v>
+        <v>1620</v>
       </c>
       <c r="C95" s="44">
         <v>1</v>
       </c>
       <c r="D95" s="44" t="s">
-        <v>1567</v>
+        <v>1682</v>
       </c>
       <c r="E95" s="45" t="s">
         <v>1211</v>
       </c>
       <c r="F95" s="43" t="s">
-        <v>1545</v>
+        <v>1683</v>
       </c>
       <c r="G95" s="44">
         <v>3</v>
       </c>
       <c r="H95" s="44" t="s">
-        <v>1568</v>
+        <v>1685</v>
       </c>
       <c r="I95" s="91" t="s">
-        <v>1672</v>
+        <v>1702</v>
       </c>
     </row>
     <row r="96" spans="1:9" s="44" customFormat="1" x14ac:dyDescent="0.35">
@@ -9273,25 +9278,25 @@
         <v>4</v>
       </c>
       <c r="B96" s="43" t="s">
-        <v>1640</v>
+        <v>1545</v>
       </c>
       <c r="C96" s="44">
         <v>1</v>
       </c>
       <c r="D96" s="44" t="s">
-        <v>1691</v>
+        <v>1567</v>
       </c>
       <c r="E96" s="45" t="s">
         <v>1211</v>
       </c>
       <c r="F96" s="43" t="s">
-        <v>1640</v>
+        <v>1545</v>
       </c>
       <c r="G96" s="44">
         <v>3</v>
       </c>
       <c r="H96" s="44" t="s">
-        <v>1692</v>
+        <v>1568</v>
       </c>
       <c r="I96" s="91" t="s">
         <v>1672</v>
@@ -9302,28 +9307,28 @@
         <v>4</v>
       </c>
       <c r="B97" s="43" t="s">
-        <v>1547</v>
+        <v>1640</v>
       </c>
       <c r="C97" s="44">
         <v>1</v>
       </c>
       <c r="D97" s="44" t="s">
-        <v>1562</v>
+        <v>1691</v>
       </c>
       <c r="E97" s="45" t="s">
         <v>1211</v>
       </c>
       <c r="F97" s="43" t="s">
-        <v>1547</v>
+        <v>1640</v>
       </c>
       <c r="G97" s="44">
         <v>3</v>
       </c>
       <c r="H97" s="44" t="s">
-        <v>1563</v>
+        <v>1692</v>
       </c>
       <c r="I97" s="91" t="s">
-        <v>1673</v>
+        <v>1672</v>
       </c>
     </row>
     <row r="98" spans="1:9" s="44" customFormat="1" x14ac:dyDescent="0.35">
@@ -9331,25 +9336,25 @@
         <v>4</v>
       </c>
       <c r="B98" s="43" t="s">
-        <v>1637</v>
+        <v>1547</v>
       </c>
       <c r="C98" s="44">
         <v>1</v>
       </c>
       <c r="D98" s="44" t="s">
-        <v>1695</v>
+        <v>1562</v>
       </c>
       <c r="E98" s="45" t="s">
         <v>1211</v>
       </c>
       <c r="F98" s="43" t="s">
-        <v>1637</v>
+        <v>1547</v>
       </c>
       <c r="G98" s="44">
         <v>3</v>
       </c>
       <c r="H98" s="44" t="s">
-        <v>1696</v>
+        <v>1563</v>
       </c>
       <c r="I98" s="91" t="s">
         <v>1673</v>
@@ -9360,28 +9365,28 @@
         <v>4</v>
       </c>
       <c r="B99" s="43" t="s">
-        <v>1621</v>
+        <v>1637</v>
       </c>
       <c r="C99" s="44">
         <v>1</v>
       </c>
       <c r="D99" s="44" t="s">
-        <v>1693</v>
+        <v>1695</v>
       </c>
       <c r="E99" s="45" t="s">
         <v>1211</v>
       </c>
       <c r="F99" s="43" t="s">
-        <v>1621</v>
+        <v>1637</v>
       </c>
       <c r="G99" s="44">
         <v>3</v>
       </c>
       <c r="H99" s="44" t="s">
-        <v>1694</v>
+        <v>1696</v>
       </c>
       <c r="I99" s="91" t="s">
-        <v>1703</v>
+        <v>1673</v>
       </c>
     </row>
     <row r="100" spans="1:9" s="44" customFormat="1" x14ac:dyDescent="0.35">
@@ -9389,28 +9394,28 @@
         <v>4</v>
       </c>
       <c r="B100" s="43" t="s">
-        <v>1595</v>
+        <v>1621</v>
       </c>
       <c r="C100" s="44">
         <v>1</v>
       </c>
       <c r="D100" s="44" t="s">
-        <v>1596</v>
+        <v>1693</v>
       </c>
       <c r="E100" s="45" t="s">
         <v>1211</v>
       </c>
       <c r="F100" s="43" t="s">
-        <v>1598</v>
+        <v>1621</v>
       </c>
       <c r="G100" s="44">
         <v>3</v>
       </c>
       <c r="H100" s="44" t="s">
-        <v>1599</v>
+        <v>1694</v>
       </c>
       <c r="I100" s="91" t="s">
-        <v>1704</v>
+        <v>1703</v>
       </c>
     </row>
     <row r="101" spans="1:9" s="44" customFormat="1" x14ac:dyDescent="0.35">
@@ -9418,32 +9423,61 @@
         <v>4</v>
       </c>
       <c r="B101" s="43" t="s">
-        <v>604</v>
+        <v>1595</v>
       </c>
       <c r="C101" s="44">
         <v>1</v>
       </c>
       <c r="D101" s="44" t="s">
-        <v>639</v>
+        <v>1596</v>
       </c>
       <c r="E101" s="45" t="s">
         <v>1211</v>
       </c>
       <c r="F101" s="43" t="s">
+        <v>1598</v>
+      </c>
+      <c r="G101" s="44">
+        <v>3</v>
+      </c>
+      <c r="H101" s="44" t="s">
+        <v>1599</v>
+      </c>
+      <c r="I101" s="91" t="s">
+        <v>1704</v>
+      </c>
+    </row>
+    <row r="102" spans="1:9" s="44" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A102" s="42">
+        <v>4</v>
+      </c>
+      <c r="B102" s="43" t="s">
         <v>604</v>
       </c>
-      <c r="G101" s="44">
-        <v>3</v>
-      </c>
-      <c r="H101" s="44" t="s">
+      <c r="C102" s="44">
+        <v>1</v>
+      </c>
+      <c r="D102" s="44" t="s">
+        <v>639</v>
+      </c>
+      <c r="E102" s="45" t="s">
+        <v>1211</v>
+      </c>
+      <c r="F102" s="43" t="s">
+        <v>604</v>
+      </c>
+      <c r="G102" s="44">
+        <v>3</v>
+      </c>
+      <c r="H102" s="44" t="s">
         <v>644</v>
       </c>
-      <c r="I101" s="91" t="s">
+      <c r="I102" s="91" t="s">
         <v>1614</v>
       </c>
     </row>
-    <row r="102" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="B102" s="33"/>
+    <row r="103" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="B103" s="33"/>
     </row>
   </sheetData>
   <hyperlinks>

</xml_diff>